<commit_message>
added routes 4,5,6 and made f function in main
</commit_message>
<xml_diff>
--- a/Sushrut/currentSchedule.xlsx
+++ b/Sushrut/currentSchedule.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Temp\Project\TumTum-Schedule\Sushrut\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7650"/>
   </bookViews>
@@ -15,11 +10,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="tumtum_sche_1" localSheetId="0">Sheet1!$A$1:$U$16</definedName>
+    <definedName name="tumtum_sche_1" localSheetId="0">Sheet1!$A$1:$V$16</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -57,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="26">
   <si>
     <t>Via</t>
   </si>
@@ -128,14 +123,20 @@
     <t>StartDelay</t>
   </si>
   <si>
-    <t>StartTimingsfromthestartingpoint</t>
+    <t>Start Timings from the starting point</t>
+  </si>
+  <si>
+    <t>Frequency from 8:10 to 8:45</t>
+  </si>
+  <si>
+    <t>Distance Travelled in meters</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,10 +165,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -232,7 +234,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -267,7 +269,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -444,70 +446,76 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CQ16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:CR18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="Z18" sqref="Z18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.875" customWidth="1"/>
-    <col min="6" max="6" width="7.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.75" bestFit="1" customWidth="1"/>
-    <col min="11" max="18" width="6.875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.875" customWidth="1"/>
-    <col min="20" max="20" width="6.875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.875" customWidth="1"/>
-    <col min="23" max="23" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="22.75" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="27" max="39" width="6.875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="13" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="22.75" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="5.375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="6.875" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="48" max="58" width="6.875" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="13" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="6.875" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="22.75" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="65" max="76" width="6.875" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="2.875" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="13" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="6" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="22.75" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="5.375" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="84" max="94" width="6.875" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="5.28515625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" customWidth="1"/>
+    <col min="9" max="10" width="8.5703125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" hidden="1" customWidth="1"/>
+    <col min="14" max="15" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="8" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="8.5703125" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="8.7109375" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="8.42578125" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="9.5703125" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="7.85546875" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="6.85546875" customWidth="1"/>
+    <col min="24" max="24" width="9.5703125" customWidth="1"/>
+    <col min="25" max="25" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.28515625" customWidth="1"/>
+    <col min="27" max="27" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="40" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="13" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="49" max="59" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="13" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="66" max="77" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="13" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="6" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="85" max="95" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="7.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:96">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -529,10 +537,10 @@
       <c r="G1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="2"/>
+      <c r="I1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -543,9 +551,14 @@
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="X1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1"/>
       <c r="AB1" s="2"/>
       <c r="AC1" s="2"/>
       <c r="AD1" s="2"/>
@@ -557,9 +570,9 @@
       <c r="AJ1" s="2"/>
       <c r="AK1" s="2"/>
       <c r="AL1" s="2"/>
-      <c r="AR1" s="1"/>
+      <c r="AM1" s="2"/>
       <c r="AS1" s="1"/>
-      <c r="AT1" s="2"/>
+      <c r="AT1" s="1"/>
       <c r="AU1" s="2"/>
       <c r="AV1" s="2"/>
       <c r="AW1" s="2"/>
@@ -571,9 +584,9 @@
       <c r="BC1" s="2"/>
       <c r="BD1" s="2"/>
       <c r="BE1" s="2"/>
-      <c r="BK1" s="1"/>
+      <c r="BF1" s="2"/>
       <c r="BL1" s="1"/>
-      <c r="BM1" s="2"/>
+      <c r="BM1" s="1"/>
       <c r="BN1" s="2"/>
       <c r="BO1" s="2"/>
       <c r="BP1" s="2"/>
@@ -585,9 +598,9 @@
       <c r="BV1" s="2"/>
       <c r="BW1" s="2"/>
       <c r="BX1" s="2"/>
-      <c r="CD1" s="1"/>
+      <c r="BY1" s="2"/>
       <c r="CE1" s="1"/>
-      <c r="CF1" s="2"/>
+      <c r="CF1" s="1"/>
       <c r="CG1" s="2"/>
       <c r="CH1" s="2"/>
       <c r="CI1" s="2"/>
@@ -599,8 +612,9 @@
       <c r="CO1" s="2"/>
       <c r="CP1" s="2"/>
       <c r="CQ1" s="2"/>
+      <c r="CR1" s="2"/>
     </row>
-    <row r="2" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:96">
       <c r="A2">
         <v>50</v>
       </c>
@@ -622,45 +636,52 @@
       <c r="G2" s="2">
         <v>0</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="2"/>
+      <c r="I2" s="2">
         <v>0.33333333333333331</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <v>0.34050925925925929</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <v>0.34768518518518521</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <v>0.35486111111111113</v>
       </c>
-      <c r="L2" s="2">
+      <c r="M2" s="2">
         <v>0.36203703703703699</v>
       </c>
-      <c r="M2" s="2">
+      <c r="N2" s="2">
         <v>0.36921296296296297</v>
       </c>
-      <c r="N2" s="2">
+      <c r="O2" s="2">
         <v>0.37638888888888888</v>
       </c>
-      <c r="O2" s="2">
+      <c r="P2" s="2">
         <v>0.3835648148148148</v>
       </c>
-      <c r="P2" s="2">
+      <c r="Q2" s="2">
         <v>0.39074074074074078</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="R2" s="2">
         <v>0.3979166666666667</v>
       </c>
-      <c r="R2" s="2">
+      <c r="S2" s="2">
         <v>0.40509259259259256</v>
       </c>
-      <c r="S2" s="2">
+      <c r="T2" s="2">
         <v>0.41226851851851848</v>
       </c>
-      <c r="AA2" s="1"/>
+      <c r="X2">
+        <v>4</v>
+      </c>
+      <c r="Z2">
+        <f>X2*1300*2</f>
+        <v>10400</v>
+      </c>
       <c r="AB2" s="1"/>
-      <c r="AC2" s="2"/>
+      <c r="AC2" s="1"/>
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
       <c r="AF2" s="2"/>
@@ -674,8 +695,9 @@
       <c r="AN2" s="2"/>
       <c r="AO2" s="2"/>
       <c r="AP2" s="2"/>
+      <c r="AQ2" s="2"/>
     </row>
-    <row r="3" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:96">
       <c r="A3">
         <v>50</v>
       </c>
@@ -697,45 +719,52 @@
       <c r="G3" s="2">
         <v>0.125</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="2"/>
+      <c r="I3" s="2">
         <v>0.3354166666666667</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <v>0.34259259259259256</v>
       </c>
-      <c r="J3" s="2">
+      <c r="K3" s="2">
         <v>0.34976851851851848</v>
       </c>
-      <c r="K3" s="2">
+      <c r="L3" s="2">
         <v>0.35694444444444445</v>
       </c>
-      <c r="L3" s="2">
+      <c r="M3" s="2">
         <v>0.36412037037037037</v>
       </c>
-      <c r="M3" s="2">
+      <c r="N3" s="2">
         <v>0.37129629629629629</v>
       </c>
-      <c r="N3" s="2">
+      <c r="O3" s="2">
         <v>0.37847222222222227</v>
       </c>
-      <c r="O3" s="2">
+      <c r="P3" s="2">
         <v>0.38564814814814818</v>
       </c>
-      <c r="P3" s="2">
+      <c r="Q3" s="2">
         <v>0.39282407407407405</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="R3" s="2">
         <v>0.39999999999999997</v>
       </c>
-      <c r="R3" s="2">
+      <c r="S3" s="2">
         <v>0.40717592592592594</v>
       </c>
-      <c r="S3" s="2">
+      <c r="T3" s="2">
         <v>0.41435185185185186</v>
       </c>
-      <c r="AA3" s="1"/>
+      <c r="X3">
+        <v>4</v>
+      </c>
+      <c r="Z3">
+        <f t="shared" ref="Z3:Z15" si="0">X3*1300*2</f>
+        <v>10400</v>
+      </c>
       <c r="AB3" s="1"/>
-      <c r="AC3" s="2"/>
+      <c r="AC3" s="1"/>
       <c r="AD3" s="2"/>
       <c r="AE3" s="2"/>
       <c r="AF3" s="2"/>
@@ -749,9 +778,9 @@
       <c r="AN3" s="2"/>
       <c r="AO3" s="2"/>
       <c r="AP3" s="2"/>
-      <c r="AV3" s="1"/>
+      <c r="AQ3" s="2"/>
       <c r="AW3" s="1"/>
-      <c r="AX3" s="2"/>
+      <c r="AX3" s="1"/>
       <c r="AY3" s="2"/>
       <c r="AZ3" s="2"/>
       <c r="BA3" s="2"/>
@@ -765,8 +794,9 @@
       <c r="BI3" s="2"/>
       <c r="BJ3" s="2"/>
       <c r="BK3" s="2"/>
+      <c r="BL3" s="2"/>
     </row>
-    <row r="4" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:96">
       <c r="A4">
         <v>35</v>
       </c>
@@ -788,45 +818,52 @@
       <c r="G4" s="1">
         <v>0.20833333333333334</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1"/>
+      <c r="I4" s="2">
         <v>0.33680555555555558</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="2">
         <v>0.3439814814814815</v>
       </c>
-      <c r="J4" s="2">
+      <c r="K4" s="2">
         <v>0.35115740740740736</v>
       </c>
-      <c r="K4" s="2">
+      <c r="L4" s="2">
         <v>0.35833333333333334</v>
       </c>
-      <c r="L4" s="2">
+      <c r="M4" s="2">
         <v>0.36550925925925926</v>
       </c>
-      <c r="M4" s="2">
+      <c r="N4" s="2">
         <v>0.37268518518518517</v>
       </c>
-      <c r="N4" s="2">
+      <c r="O4" s="2">
         <v>0.37986111111111115</v>
       </c>
-      <c r="O4" s="2">
+      <c r="P4" s="2">
         <v>0.38703703703703707</v>
       </c>
-      <c r="P4" s="2">
+      <c r="Q4" s="2">
         <v>0.39421296296296293</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="R4" s="2">
         <v>0.40138888888888885</v>
       </c>
-      <c r="R4" s="2">
+      <c r="S4" s="2">
         <v>0.40856481481481483</v>
       </c>
-      <c r="S4" s="2">
+      <c r="T4" s="2">
         <v>0.41574074074074074</v>
       </c>
-      <c r="AA4" s="1"/>
+      <c r="X4">
+        <v>4</v>
+      </c>
+      <c r="Z4">
+        <f t="shared" si="0"/>
+        <v>10400</v>
+      </c>
       <c r="AB4" s="1"/>
-      <c r="AC4" s="2"/>
+      <c r="AC4" s="1"/>
       <c r="AD4" s="2"/>
       <c r="AE4" s="2"/>
       <c r="AF4" s="2"/>
@@ -840,9 +877,9 @@
       <c r="AN4" s="2"/>
       <c r="AO4" s="2"/>
       <c r="AP4" s="2"/>
-      <c r="AV4" s="1"/>
+      <c r="AQ4" s="2"/>
       <c r="AW4" s="1"/>
-      <c r="AX4" s="2"/>
+      <c r="AX4" s="1"/>
       <c r="AY4" s="2"/>
       <c r="AZ4" s="2"/>
       <c r="BA4" s="2"/>
@@ -856,8 +893,9 @@
       <c r="BI4" s="2"/>
       <c r="BJ4" s="2"/>
       <c r="BK4" s="2"/>
+      <c r="BL4" s="2"/>
     </row>
-    <row r="5" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:96">
       <c r="A5">
         <v>50</v>
       </c>
@@ -879,45 +917,52 @@
       <c r="G5" s="1">
         <v>0.375</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1"/>
+      <c r="I5" s="2">
         <v>0.33958333333333335</v>
       </c>
-      <c r="I5" s="2">
+      <c r="J5" s="2">
         <v>0.34675925925925927</v>
       </c>
-      <c r="J5" s="2">
+      <c r="K5" s="2">
         <v>0.35393518518518513</v>
       </c>
-      <c r="K5" s="2">
+      <c r="L5" s="2">
         <v>0.3611111111111111</v>
       </c>
-      <c r="L5" s="2">
+      <c r="M5" s="2">
         <v>0.36828703703703702</v>
       </c>
-      <c r="M5" s="2">
+      <c r="N5" s="2">
         <v>0.37546296296296294</v>
       </c>
-      <c r="N5" s="2">
+      <c r="O5" s="2">
         <v>0.38263888888888892</v>
       </c>
-      <c r="O5" s="2">
+      <c r="P5" s="2">
         <v>0.38981481481481484</v>
       </c>
-      <c r="P5" s="2">
+      <c r="Q5" s="2">
         <v>0.39699074074074076</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="R5" s="2">
         <v>0.40416666666666662</v>
       </c>
-      <c r="R5" s="2">
+      <c r="S5" s="2">
         <v>0.41134259259259259</v>
       </c>
-      <c r="S5" s="2">
+      <c r="T5" s="2">
         <v>0.41851851851851851</v>
       </c>
-      <c r="AA5" s="1"/>
+      <c r="X5">
+        <v>3</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" si="0"/>
+        <v>7800</v>
+      </c>
       <c r="AB5" s="1"/>
-      <c r="AC5" s="2"/>
+      <c r="AC5" s="1"/>
       <c r="AD5" s="2"/>
       <c r="AE5" s="2"/>
       <c r="AF5" s="2"/>
@@ -931,9 +976,9 @@
       <c r="AN5" s="2"/>
       <c r="AO5" s="2"/>
       <c r="AP5" s="2"/>
-      <c r="AV5" s="1"/>
+      <c r="AQ5" s="2"/>
       <c r="AW5" s="1"/>
-      <c r="AX5" s="2"/>
+      <c r="AX5" s="1"/>
       <c r="AY5" s="2"/>
       <c r="AZ5" s="2"/>
       <c r="BA5" s="2"/>
@@ -947,8 +992,9 @@
       <c r="BI5" s="2"/>
       <c r="BJ5" s="2"/>
       <c r="BK5" s="2"/>
+      <c r="BL5" s="2"/>
     </row>
-    <row r="6" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:96">
       <c r="A6">
         <v>35</v>
       </c>
@@ -970,50 +1016,58 @@
       <c r="G6" s="1">
         <v>0</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="1"/>
+      <c r="I6" s="2">
         <v>0.33333333333333331</v>
       </c>
-      <c r="I6" s="2">
+      <c r="J6" s="2">
         <v>0.33946759259259257</v>
       </c>
-      <c r="J6" s="2">
+      <c r="K6" s="2">
         <v>0.34560185185185183</v>
       </c>
-      <c r="K6" s="2">
+      <c r="L6" s="2">
         <v>0.35173611111111108</v>
       </c>
-      <c r="L6" s="2">
+      <c r="M6" s="2">
         <v>0.35787037037037034</v>
       </c>
-      <c r="M6" s="2">
+      <c r="N6" s="2">
         <v>0.36400462962962959</v>
       </c>
-      <c r="N6" s="2">
+      <c r="O6" s="2">
         <v>0.37013888888888885</v>
       </c>
-      <c r="O6" s="2">
+      <c r="P6" s="2">
         <v>0.37627314814814811</v>
       </c>
-      <c r="P6" s="2">
+      <c r="Q6" s="2">
         <v>0.38240740740740736</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="R6" s="2">
         <v>0.38854166666666662</v>
       </c>
-      <c r="R6" s="2">
+      <c r="S6" s="2">
         <v>0.39467592592592587</v>
       </c>
-      <c r="S6" s="2">
+      <c r="T6" s="2">
         <v>0.40081018518518513</v>
       </c>
-      <c r="T6" s="2">
+      <c r="U6" s="2">
         <v>0.4069444444444445</v>
       </c>
-      <c r="U6" s="2">
+      <c r="V6" s="2">
         <v>0.41307870370370375</v>
       </c>
+      <c r="X6" s="3">
+        <v>4</v>
+      </c>
+      <c r="Z6">
+        <f>X6*1170*2</f>
+        <v>9360</v>
+      </c>
     </row>
-    <row r="7" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:96">
       <c r="A7">
         <v>50</v>
       </c>
@@ -1035,50 +1089,58 @@
       <c r="G7" s="1">
         <v>0.125</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="1"/>
+      <c r="I7" s="2">
         <v>0.3354166666666667</v>
       </c>
-      <c r="I7" s="2">
+      <c r="J7" s="2">
         <v>0.34155092592592595</v>
       </c>
-      <c r="J7" s="2">
+      <c r="K7" s="2">
         <v>0.34768518518518521</v>
       </c>
-      <c r="K7" s="2">
+      <c r="L7" s="2">
         <v>0.35381944444444446</v>
       </c>
-      <c r="L7" s="2">
+      <c r="M7" s="2">
         <v>0.35995370370370372</v>
       </c>
-      <c r="M7" s="2">
+      <c r="N7" s="2">
         <v>0.36608796296296298</v>
       </c>
-      <c r="N7" s="2">
+      <c r="O7" s="2">
         <v>0.37222222222222223</v>
       </c>
-      <c r="O7" s="2">
+      <c r="P7" s="2">
         <v>0.37835648148148149</v>
       </c>
-      <c r="P7" s="2">
+      <c r="Q7" s="2">
         <v>0.38449074074074074</v>
       </c>
-      <c r="Q7" s="2">
+      <c r="R7" s="2">
         <v>0.390625</v>
       </c>
-      <c r="R7" s="2">
+      <c r="S7" s="2">
         <v>0.39675925925925926</v>
       </c>
-      <c r="S7" s="2">
+      <c r="T7" s="2">
         <v>0.40289351851851851</v>
       </c>
-      <c r="T7" s="2">
+      <c r="U7" s="2">
         <v>0.40902777777777777</v>
       </c>
-      <c r="U7" s="2">
+      <c r="V7" s="2">
         <v>0.41516203703703702</v>
       </c>
+      <c r="X7" s="3">
+        <v>4</v>
+      </c>
+      <c r="Z7">
+        <f>X7*1170*2</f>
+        <v>9360</v>
+      </c>
     </row>
-    <row r="8" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:96">
       <c r="A8">
         <v>30</v>
       </c>
@@ -1100,50 +1162,58 @@
       <c r="G8" s="1">
         <v>0</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="1"/>
+      <c r="I8" s="2">
         <v>0.33333333333333331</v>
       </c>
-      <c r="I8" s="2">
+      <c r="J8" s="2">
         <v>0.33958333333333335</v>
       </c>
-      <c r="J8" s="2">
+      <c r="K8" s="2">
         <v>0.34583333333333338</v>
       </c>
-      <c r="K8" s="2">
+      <c r="L8" s="2">
         <v>0.3520833333333333</v>
       </c>
-      <c r="L8" s="2">
+      <c r="M8" s="2">
         <v>0.35833333333333334</v>
       </c>
-      <c r="M8" s="2">
+      <c r="N8" s="2">
         <v>0.36458333333333331</v>
       </c>
-      <c r="N8" s="2">
+      <c r="O8" s="2">
         <v>0.37083333333333335</v>
       </c>
-      <c r="O8" s="2">
+      <c r="P8" s="2">
         <v>0.37708333333333338</v>
       </c>
-      <c r="P8" s="2">
+      <c r="Q8" s="2">
         <v>0.3833333333333333</v>
       </c>
-      <c r="Q8" s="2">
+      <c r="R8" s="2">
         <v>0.38958333333333334</v>
       </c>
-      <c r="R8" s="2">
+      <c r="S8" s="2">
         <v>0.39583333333333331</v>
       </c>
-      <c r="S8" s="2">
+      <c r="T8" s="2">
         <v>0.40208333333333335</v>
       </c>
-      <c r="T8" s="2">
+      <c r="U8" s="2">
         <v>0.40833333333333338</v>
       </c>
-      <c r="U8" s="2">
+      <c r="V8" s="2">
         <v>0.4145833333333333</v>
       </c>
+      <c r="X8" s="3">
+        <v>4</v>
+      </c>
+      <c r="Z8">
+        <f>X8*(990 + 1170)</f>
+        <v>8640</v>
+      </c>
     </row>
-    <row r="9" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:96">
       <c r="A9">
         <v>30</v>
       </c>
@@ -1165,50 +1235,58 @@
       <c r="G9" s="1">
         <v>0.125</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="1"/>
+      <c r="I9" s="2">
         <v>0.3354166666666667</v>
       </c>
-      <c r="I9" s="2">
+      <c r="J9" s="2">
         <v>0.34166666666666662</v>
       </c>
-      <c r="J9" s="2">
+      <c r="K9" s="2">
         <v>0.34791666666666665</v>
       </c>
-      <c r="K9" s="2">
+      <c r="L9" s="2">
         <v>0.35416666666666669</v>
       </c>
-      <c r="L9" s="2">
+      <c r="M9" s="2">
         <v>0.36041666666666666</v>
       </c>
-      <c r="M9" s="2">
+      <c r="N9" s="2">
         <v>0.3666666666666667</v>
       </c>
-      <c r="N9" s="2">
+      <c r="O9" s="2">
         <v>0.37291666666666662</v>
       </c>
-      <c r="O9" s="2">
+      <c r="P9" s="2">
         <v>0.37916666666666665</v>
       </c>
-      <c r="P9" s="2">
+      <c r="Q9" s="2">
         <v>0.38541666666666669</v>
       </c>
-      <c r="Q9" s="2">
+      <c r="R9" s="2">
         <v>0.39166666666666666</v>
       </c>
-      <c r="R9" s="2">
+      <c r="S9" s="2">
         <v>0.3979166666666667</v>
       </c>
-      <c r="S9" s="2">
+      <c r="T9" s="2">
         <v>0.40416666666666662</v>
       </c>
-      <c r="T9" s="2">
+      <c r="U9" s="2">
         <v>0.41041666666666665</v>
       </c>
-      <c r="U9" s="2">
+      <c r="V9" s="2">
         <v>0.41666666666666669</v>
       </c>
+      <c r="X9" s="3">
+        <v>4</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" ref="Z9:Z13" si="1">X9*(990 + 1170)</f>
+        <v>8640</v>
+      </c>
     </row>
-    <row r="10" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:96">
       <c r="A10">
         <v>50</v>
       </c>
@@ -1230,50 +1308,58 @@
       <c r="G10" s="1">
         <v>0.20833333333333334</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="1"/>
+      <c r="I10" s="2">
         <v>0.33680555555555558</v>
       </c>
-      <c r="I10" s="2">
+      <c r="J10" s="2">
         <v>0.3430555555555555</v>
       </c>
-      <c r="J10" s="2">
+      <c r="K10" s="2">
         <v>0.34930555555555554</v>
       </c>
-      <c r="K10" s="2">
+      <c r="L10" s="2">
         <v>0.35555555555555557</v>
       </c>
-      <c r="L10" s="2">
+      <c r="M10" s="2">
         <v>0.36180555555555555</v>
       </c>
-      <c r="M10" s="2">
+      <c r="N10" s="2">
         <v>0.36805555555555558</v>
       </c>
-      <c r="N10" s="2">
+      <c r="O10" s="2">
         <v>0.3743055555555555</v>
       </c>
-      <c r="O10" s="2">
+      <c r="P10" s="2">
         <v>0.38055555555555554</v>
       </c>
-      <c r="P10" s="2">
+      <c r="Q10" s="2">
         <v>0.38680555555555557</v>
       </c>
-      <c r="Q10" s="2">
+      <c r="R10" s="2">
         <v>0.39305555555555555</v>
       </c>
-      <c r="R10" s="2">
+      <c r="S10" s="2">
         <v>0.39930555555555558</v>
       </c>
-      <c r="S10" s="2">
+      <c r="T10" s="2">
         <v>0.4055555555555555</v>
       </c>
-      <c r="T10" s="2">
+      <c r="U10" s="2">
         <v>0.41180555555555554</v>
       </c>
-      <c r="U10" s="2">
+      <c r="V10" s="2">
         <v>0.41805555555555557</v>
       </c>
+      <c r="X10" s="3">
+        <v>4</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" si="1"/>
+        <v>8640</v>
+      </c>
     </row>
-    <row r="11" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:96">
       <c r="A11">
         <v>30</v>
       </c>
@@ -1295,50 +1381,58 @@
       <c r="G11" s="1">
         <v>0</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="1"/>
+      <c r="I11" s="2">
         <v>0.33333333333333331</v>
       </c>
-      <c r="I11" s="2">
+      <c r="J11" s="2">
         <v>0.33946759259259257</v>
       </c>
-      <c r="J11" s="2">
+      <c r="K11" s="2">
         <v>0.34560185185185183</v>
       </c>
-      <c r="K11" s="2">
+      <c r="L11" s="2">
         <v>0.35173611111111108</v>
       </c>
-      <c r="L11" s="2">
+      <c r="M11" s="2">
         <v>0.35787037037037034</v>
       </c>
-      <c r="M11" s="2">
+      <c r="N11" s="2">
         <v>0.36400462962962959</v>
       </c>
-      <c r="N11" s="2">
+      <c r="O11" s="2">
         <v>0.37013888888888885</v>
       </c>
-      <c r="O11" s="2">
+      <c r="P11" s="2">
         <v>0.37627314814814811</v>
       </c>
-      <c r="P11" s="2">
+      <c r="Q11" s="2">
         <v>0.38240740740740736</v>
       </c>
-      <c r="Q11" s="2">
+      <c r="R11" s="2">
         <v>0.38854166666666662</v>
       </c>
-      <c r="R11" s="2">
+      <c r="S11" s="2">
         <v>0.39467592592592587</v>
       </c>
-      <c r="S11" s="2">
+      <c r="T11" s="2">
         <v>0.40081018518518513</v>
       </c>
-      <c r="T11" s="2">
+      <c r="U11" s="2">
         <v>0.4069444444444445</v>
       </c>
-      <c r="U11" s="2">
+      <c r="V11" s="2">
         <v>0.41307870370370375</v>
       </c>
+      <c r="X11" s="3">
+        <v>4</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" si="1"/>
+        <v>8640</v>
+      </c>
     </row>
-    <row r="12" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:96">
       <c r="A12">
         <v>30</v>
       </c>
@@ -1360,50 +1454,58 @@
       <c r="G12" s="1">
         <v>0.125</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="1"/>
+      <c r="I12" s="2">
         <v>0.3354166666666667</v>
       </c>
-      <c r="I12" s="2">
+      <c r="J12" s="2">
         <v>0.34155092592592595</v>
       </c>
-      <c r="J12" s="2">
+      <c r="K12" s="2">
         <v>0.34768518518518521</v>
       </c>
-      <c r="K12" s="2">
+      <c r="L12" s="2">
         <v>0.35381944444444446</v>
       </c>
-      <c r="L12" s="2">
+      <c r="M12" s="2">
         <v>0.35995370370370372</v>
       </c>
-      <c r="M12" s="2">
+      <c r="N12" s="2">
         <v>0.36608796296296298</v>
       </c>
-      <c r="N12" s="2">
+      <c r="O12" s="2">
         <v>0.37222222222222223</v>
       </c>
-      <c r="O12" s="2">
+      <c r="P12" s="2">
         <v>0.37835648148148149</v>
       </c>
-      <c r="P12" s="2">
+      <c r="Q12" s="2">
         <v>0.38449074074074074</v>
       </c>
-      <c r="Q12" s="2">
+      <c r="R12" s="2">
         <v>0.390625</v>
       </c>
-      <c r="R12" s="2">
+      <c r="S12" s="2">
         <v>0.39675925925925926</v>
       </c>
-      <c r="S12" s="2">
+      <c r="T12" s="2">
         <v>0.40289351851851851</v>
       </c>
-      <c r="T12" s="2">
+      <c r="U12" s="2">
         <v>0.40902777777777777</v>
       </c>
-      <c r="U12" s="2">
+      <c r="V12" s="2">
         <v>0.41516203703703702</v>
       </c>
+      <c r="X12" s="3">
+        <v>4</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" si="1"/>
+        <v>8640</v>
+      </c>
     </row>
-    <row r="13" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:96">
       <c r="A13">
         <v>50</v>
       </c>
@@ -1425,50 +1527,58 @@
       <c r="G13" s="1">
         <v>0.20833333333333334</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="1"/>
+      <c r="I13" s="2">
         <v>0.33680555555555558</v>
       </c>
-      <c r="I13" s="2">
+      <c r="J13" s="2">
         <v>0.34293981481481484</v>
       </c>
-      <c r="J13" s="2">
+      <c r="K13" s="2">
         <v>0.34907407407407409</v>
       </c>
-      <c r="K13" s="2">
+      <c r="L13" s="2">
         <v>0.35520833333333335</v>
       </c>
-      <c r="L13" s="2">
+      <c r="M13" s="2">
         <v>0.3613425925925926</v>
       </c>
-      <c r="M13" s="2">
+      <c r="N13" s="2">
         <v>0.36747685185185186</v>
       </c>
-      <c r="N13" s="2">
+      <c r="O13" s="2">
         <v>0.37361111111111112</v>
       </c>
-      <c r="O13" s="2">
+      <c r="P13" s="2">
         <v>0.37974537037037037</v>
       </c>
-      <c r="P13" s="2">
+      <c r="Q13" s="2">
         <v>0.38587962962962963</v>
       </c>
-      <c r="Q13" s="2">
+      <c r="R13" s="2">
         <v>0.39201388888888888</v>
       </c>
-      <c r="R13" s="2">
+      <c r="S13" s="2">
         <v>0.39814814814814814</v>
       </c>
-      <c r="S13" s="2">
+      <c r="T13" s="2">
         <v>0.4042824074074074</v>
       </c>
-      <c r="T13" s="2">
+      <c r="U13" s="2">
         <v>0.41041666666666665</v>
       </c>
-      <c r="U13" s="2">
+      <c r="V13" s="2">
         <v>0.41655092592592591</v>
       </c>
+      <c r="X13" s="3">
+        <v>4</v>
+      </c>
+      <c r="Z13">
+        <f t="shared" si="1"/>
+        <v>8640</v>
+      </c>
     </row>
-    <row r="14" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:96">
       <c r="A14">
         <v>30</v>
       </c>
@@ -1490,50 +1600,58 @@
       <c r="G14" s="1">
         <v>0</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="1"/>
+      <c r="I14" s="2">
         <v>0.33333333333333331</v>
       </c>
-      <c r="I14" s="2">
+      <c r="J14" s="2">
         <v>0.33940972222222227</v>
       </c>
-      <c r="J14" s="2">
+      <c r="K14" s="2">
         <v>0.3454861111111111</v>
       </c>
-      <c r="K14" s="2">
+      <c r="L14" s="2">
         <v>0.3515625</v>
       </c>
-      <c r="L14" s="2">
+      <c r="M14" s="2">
         <v>0.3576388888888889</v>
       </c>
-      <c r="M14" s="2">
+      <c r="N14" s="2">
         <v>0.36371527777777773</v>
       </c>
-      <c r="N14" s="2">
+      <c r="O14" s="2">
         <v>0.36979166666666669</v>
       </c>
-      <c r="O14" s="2">
+      <c r="P14" s="2">
         <v>0.37586805555555558</v>
       </c>
-      <c r="P14" s="2">
+      <c r="Q14" s="2">
         <v>0.38194444444444442</v>
       </c>
-      <c r="Q14" s="2">
+      <c r="R14" s="2">
         <v>0.38802083333333331</v>
       </c>
-      <c r="R14" s="2">
+      <c r="S14" s="2">
         <v>0.39409722222222227</v>
       </c>
-      <c r="S14" s="2">
+      <c r="T14" s="2">
         <v>0.4001736111111111</v>
       </c>
-      <c r="T14" s="2">
+      <c r="U14" s="2">
         <v>0.40625</v>
       </c>
-      <c r="U14" s="2">
+      <c r="V14" s="2">
         <v>0.4123263888888889</v>
       </c>
+      <c r="X14" s="3">
+        <v>4</v>
+      </c>
+      <c r="Z14">
+        <f>X14*880*2</f>
+        <v>7040</v>
+      </c>
     </row>
-    <row r="15" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:96">
       <c r="A15">
         <v>30</v>
       </c>
@@ -1555,50 +1673,58 @@
       <c r="G15" s="1">
         <v>0.125</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="1"/>
+      <c r="I15" s="2">
         <v>0.3354166666666667</v>
       </c>
-      <c r="I15" s="2">
+      <c r="J15" s="2">
         <v>0.34149305555555554</v>
       </c>
-      <c r="J15" s="2">
+      <c r="K15" s="2">
         <v>0.34756944444444443</v>
       </c>
-      <c r="K15" s="2">
+      <c r="L15" s="2">
         <v>0.35364583333333338</v>
       </c>
-      <c r="L15" s="2">
+      <c r="M15" s="2">
         <v>0.35972222222222222</v>
       </c>
-      <c r="M15" s="2">
+      <c r="N15" s="2">
         <v>0.36579861111111112</v>
       </c>
-      <c r="N15" s="2">
+      <c r="O15" s="2">
         <v>0.37187500000000001</v>
       </c>
-      <c r="O15" s="2">
+      <c r="P15" s="2">
         <v>0.37795138888888885</v>
       </c>
-      <c r="P15" s="2">
+      <c r="Q15" s="2">
         <v>0.3840277777777778</v>
       </c>
-      <c r="Q15" s="2">
+      <c r="R15" s="2">
         <v>0.3901041666666667</v>
       </c>
-      <c r="R15" s="2">
+      <c r="S15" s="2">
         <v>0.39618055555555554</v>
       </c>
-      <c r="S15" s="2">
+      <c r="T15" s="2">
         <v>0.40225694444444443</v>
       </c>
-      <c r="T15" s="2">
+      <c r="U15" s="2">
         <v>0.40833333333333338</v>
       </c>
-      <c r="U15" s="2">
+      <c r="V15" s="2">
         <v>0.41440972222222222</v>
       </c>
+      <c r="X15" s="3">
+        <v>4</v>
+      </c>
+      <c r="Z15">
+        <f t="shared" ref="Z15:Z16" si="2">X15*880*2</f>
+        <v>7040</v>
+      </c>
     </row>
-    <row r="16" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:96">
       <c r="A16">
         <v>50</v>
       </c>
@@ -1620,50 +1746,65 @@
       <c r="G16" s="1">
         <v>0.20833333333333334</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="1"/>
+      <c r="I16" s="2">
         <v>0.33680555555555558</v>
       </c>
-      <c r="I16" s="2">
+      <c r="J16" s="2">
         <v>0.34288194444444442</v>
       </c>
-      <c r="J16" s="2">
+      <c r="K16" s="2">
         <v>0.34895833333333331</v>
       </c>
-      <c r="K16" s="2">
+      <c r="L16" s="2">
         <v>0.35503472222222227</v>
       </c>
-      <c r="L16" s="2">
+      <c r="M16" s="2">
         <v>0.3611111111111111</v>
       </c>
-      <c r="M16" s="2">
+      <c r="N16" s="2">
         <v>0.3671875</v>
       </c>
-      <c r="N16" s="2">
+      <c r="O16" s="2">
         <v>0.3732638888888889</v>
       </c>
-      <c r="O16" s="2">
+      <c r="P16" s="2">
         <v>0.37934027777777773</v>
       </c>
-      <c r="P16" s="2">
+      <c r="Q16" s="2">
         <v>0.38541666666666669</v>
       </c>
-      <c r="Q16" s="2">
+      <c r="R16" s="2">
         <v>0.39149305555555558</v>
       </c>
-      <c r="R16" s="2">
+      <c r="S16" s="2">
         <v>0.39756944444444442</v>
       </c>
-      <c r="S16" s="2">
+      <c r="T16" s="2">
         <v>0.40364583333333331</v>
       </c>
-      <c r="T16" s="2">
+      <c r="U16" s="2">
         <v>0.40972222222222227</v>
       </c>
-      <c r="U16" s="2">
+      <c r="V16" s="2">
         <v>0.4157986111111111</v>
+      </c>
+      <c r="X16" s="3">
+        <v>4</v>
+      </c>
+      <c r="Z16">
+        <f t="shared" si="2"/>
+        <v>7040</v>
+      </c>
+    </row>
+    <row r="18" spans="26:26">
+      <c r="Z18">
+        <f>SUM(Z2:Z17)</f>
+        <v>130680</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>